<commit_message>
updated script and documentation
</commit_message>
<xml_diff>
--- a/eval_out/cross_model_flags.xlsx
+++ b/eval_out/cross_model_flags.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Cross Model Flags" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cross Model Flags" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,20 +441,25 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>MissingFromModels</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Details</t>
         </is>
@@ -468,12 +473,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>i want to sign to my account on CRA by my bank account</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ChatGPT4o</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -483,7 +488,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CRA phone number 1-800-959-8281 for individual tax enquiries | First-time users may need to provide additional information to verify identity</t>
+          <t>ChatGPT4o; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Use the same sign-in method every time you access your CRA account</t>
         </is>
       </c>
     </row>
@@ -495,22 +505,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>i want to sign to my account on CRA by my bank account</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Unique Facts</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Claude Sonnet 3.7</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Service was previously known as SecureKey Concierge | May need to provide SIN, date of birth, and tax return information for first-time registration</t>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Previously known as SecureKey Concierge</t>
         </is>
       </c>
     </row>
@@ -522,49 +537,59 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>i want to sign to my account on CRA by my bank account</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Unique Facts</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>Gemini Flash 2.o</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>AI answers response</t>
-        </is>
-      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Financial institution asks for consent to share identity information with CRA | Look for padlock icon in browser address bar for security</t>
+          <t>AI answers response; ChatGPT4o; Claude Sonnet 3.7</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Financial institution asks for consent to share identity information | Look for padlock icon in browser address bar for security</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>74aa4655e8</t>
+          <t>3feaf9d084</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>how do you find your account number when you sign into your account</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>Unique Facts</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>AI answers response</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>ChatGPT4o; Claude Sonnet 3.7; Gemini Flash 2.o</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Use the same sign-in method every time you access your CRA account</t>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Explicit statement that CRA doesn't assign single account numbers for individuals</t>
         </is>
       </c>
     </row>
@@ -576,22 +601,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>how do you find your account number when you sign into your account</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>Unique Facts</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>ChatGPT4o</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>AI answers; Claude Sonnet 3.7; Gemini Flash 2.o</t>
-        </is>
-      </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Specific phone numbers: 1-800-959-8281 for individuals, 1-800-959-5525 for businesses | Business Number format includes program identifiers like RT0001 for GST/HST</t>
+          <t>AI answers response; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Sign-in Partner method details | Program identifiers like RT0001 for GST/HST | Recovery options for forgotten credentials</t>
         </is>
       </c>
     </row>
@@ -603,22 +633,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>how do you find your account number when you sign into your account</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Claude Sonnet 3.7</t>
+          <t>Contradiction</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>AI answers; ChatGPT4o; Gemini Flash 2.o</t>
+          <t>AI answers response, ChatGPT4o, Claude Sonnet 3.7</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>SIN appears partially masked in top right section (e.g., XXX XXX 123) | Specific URL: canada.ca/my-cra-account</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Existence of separate CRA account number</t>
         </is>
       </c>
     </row>
@@ -630,76 +665,91 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>how do you find your account number when you sign into your account</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>AI answers</t>
+          <t>Contradiction</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ChatGPT4o; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+          <t>AI answers response, ChatGPT4o</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Business Number is 15 characters (not just 9 digits)</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Business Number format</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3feaf9d084</t>
+          <t>8251d93c27</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Contradiction</t>
+          <t>where do I sign in to my account? I don't want partner sign in. I do have a CRA sign in. Where do I put the information?</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>AI answers, ChatGPT4o, Claude Sonnet 3.7</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>ChatGPT4o</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>What constitutes the CRA account number</t>
+          <t>AI answers response; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Multi-factor authentication process details</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3feaf9d084</t>
+          <t>8251d93c27</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Contradiction</t>
+          <t>where do I sign in to my account? I don't want partner sign in. I do have a CRA sign in. Where do I put the information?</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>AI answers, ChatGPT4o, Claude Sonnet 3.7</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>ChatGPT4o</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Business Number format</t>
+          <t>AI answers response; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>CRA individual assistance phone number 1-800-959-8281</t>
         </is>
       </c>
     </row>
@@ -711,22 +761,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>where do I sign in to my account? I don't want partner sign in. I do have a CRA sign in. Where do I put the information?</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ChatGPT4o</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>AI answers response; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+          <t>Claude Sonnet 3.7</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>multi-factor authentication is required and involves entering a security code</t>
+          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>e-Services Helpdesk specific designation</t>
         </is>
       </c>
     </row>
@@ -738,76 +793,91 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>where do I sign in to my account? I don't want partner sign in. I do have a CRA sign in. Where do I put the information?</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ChatGPT4o</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>AI answers response; Gemini Flash 2.o</t>
+          <t>Gemini Flash 2.o</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>CRA contact number 1-800-959-8281 for individuals</t>
+          <t>AI answers response; ChatGPT4o; Claude Sonnet 3.7</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Navigation from CRA homepage through My Account button</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>8251d93c27</t>
+          <t>fe5a045281</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>I want to sign into my personal account, and only have the business account sign in</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>Unique Facts</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>Claude Sonnet 3.7</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>CRA e-Services Helpdesk contact number 1-800-959-8281</t>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Specific tax return line numbers needed for registration (line 23600, 15000) | Security code mailing timeframe (5-10 business days) | SecureKey Concierge mentioned as Sign-in Partner service name</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>8251d93c27</t>
+          <t>fe5a045281</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>I want to sign into my personal account, and only have the business account sign in</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Claude Sonnet 3.7</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>AI answers response; Gemini Flash 2.o</t>
+          <t>ChatGPT4o</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>specific options for recovering forgotten user ID or password</t>
+          <t>AI answers response; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Phone support hours (Monday-Friday 8am-8pm, Saturday 9am-5pm local time) | Multiple specific URLs for different pages</t>
         </is>
       </c>
     </row>
@@ -819,76 +889,91 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>I want to sign into my personal account, and only have the business account sign in</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Claude Sonnet 3.7</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
+          <t>Gemini Flash 2.o</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Security code mailed by CRA takes 5-10 business days | SecureKey Concierge mentioned as the Sign-in Partner service name</t>
+          <t>AI answers response; ChatGPT4o; Claude Sonnet 3.7</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Browser troubleshooting tips (clear cache/cookies, try different browser)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>fe5a045281</t>
+          <t>6466bb9c89</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>To access a client account do I sign into my cra account or theirs?</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>Unique Facts</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>ChatGPT4o</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>AI answers response; Claude Sonnet 3.7; Gemini Flash 2.o</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>CRA contact hours: Monday to Friday 8am-8pm local time, Saturday 9am-5pm local time</t>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>AUT-01 form for authorization</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>fe5a045281</t>
+          <t>6466bb9c89</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>To access a client account do I sign into my cra account or theirs?</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Gemini Flash 2.o</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>AI answers response; ChatGPT4o; Claude Sonnet 3.7</t>
+          <t>Claude Sonnet 3.7</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Suggestion to clear browser cache and cookies if experiencing issues</t>
+          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>T1013 form for individuals | RC59 form for businesses | Level 1 vs Level 2 authorization distinction</t>
         </is>
       </c>
     </row>
@@ -900,103 +985,123 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>To access a client account do I sign into my cra account or theirs?</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ChatGPT4o</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>AI answers response; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+          <t>Claude Sonnet 3.7</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Form AUT-01 as an authorization option</t>
+          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Family member authorization scenario</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>6466bb9c89</t>
+          <t>bc1cc11022</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>I want to change my sign in option from sign in partner to cra account</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Claude Sonnet 3.7</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
+          <t>AI answers</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Level 1 authorization for viewing only | Level 2 authorization for making changes | CRA e-Services Helpdesk number 1-800-959-5525</t>
+          <t>ChatGPT4o; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Must contact CRA to revoke Sign-In Partner credential (incorrect fact)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>6466bb9c89</t>
+          <t>bc1cc11022</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>I want to change my sign in option from sign in partner to cra account</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Claude Sonnet 3.7</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>AI answers response; Gemini Flash 2.o</t>
+          <t>ChatGPT4o</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Form T1013 for individuals | Form RC59 for businesses</t>
+          <t>AI answers; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Security code arrives within 10 business days | Explicitly states both sign-in methods access same account information</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>6466bb9c89</t>
+          <t>bc1cc11022</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>I want to change my sign in option from sign in partner to cra account</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Gemini Flash 2.o</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>AI answers response; ChatGPT4o; Claude Sonnet 3.7</t>
+          <t>Claude Sonnet 3.7</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Need to enter client's information like SIN or business number after logging in</t>
+          <t>AI answers; ChatGPT4o; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Personal access code (PAC) mentioned</t>
         </is>
       </c>
     </row>
@@ -1008,22 +1113,27 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>I want to change my sign in option from sign in partner to cra account</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>AI answers response</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ChatGPT4o; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+          <t>Gemini Flash 2.o</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Must contact CRA to revoke Sign-In Partner credential</t>
+          <t>AI answers; ChatGPT4o; Claude Sonnet 3.7</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Email verification process (incorrect) | Can create CRA login from within My Account (incorrect)</t>
         </is>
       </c>
     </row>
@@ -1035,22 +1145,27 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>I want to change my sign in option from sign in partner to cra account</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ChatGPT4o</t>
+          <t>Contradiction</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>AI answers response; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+          <t>AI answers, ChatGPT4o, Claude Sonnet 3.7</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Security code arrives within 10 business days | ZIP code option for non-Canadian residents</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Whether Sign-In Partner credential must be revoked</t>
         </is>
       </c>
     </row>
@@ -1062,76 +1177,91 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>I want to change my sign in option from sign in partner to cra account</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Claude Sonnet 3.7</t>
+          <t>Contradiction</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
+          <t>AI answers, ChatGPT4o, Claude Sonnet 3.7</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Personal access code (PAC) as optional requirement</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Where and how CRA user ID registration occurs</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>bc1cc11022</t>
+          <t>d0e45d52af</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>How do I access my business CRA account do you have to go to your cra ccount or go to different site</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Gemini Flash 2.o</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>AI answers response; ChatGPT4o; Claude Sonnet 3.7</t>
+          <t>ChatGPT4o</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Email verification required | Can switch from within My Account</t>
+          <t>AI answers response; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Represent a Client portal option | Form AUT-01 for authorization | BC Services Card as sign-in option</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>bc1cc11022</t>
+          <t>d0e45d52af</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Contradiction</t>
+          <t>How do I access my business CRA account do you have to go to your cra ccount or go to different site</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>AI answers response, ChatGPT4o, Claude Sonnet 3.7</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Claude Sonnet 3.7</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Process for switching from Sign-In Partner to CRA login</t>
+          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>45-day deadline to enter security code | Security code mailed to business address</t>
         </is>
       </c>
     </row>
@@ -1143,22 +1273,27 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>How do I access my business CRA account do you have to go to your cra ccount or go to different site</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ChatGPT4o</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>AI answers response; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+          <t>Gemini Flash 2.o</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Form AUT-01 can be used to authorize representatives | Provincial partner (BC Services Card) as a sign-in option</t>
+          <t>AI answers response; ChatGPT4o; Claude Sonnet 3.7</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Two-step verification details</t>
         </is>
       </c>
     </row>
@@ -1170,508 +1305,347 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>How do I access my business CRA account do you have to go to your cra ccount or go to different site</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ChatGPT4o</t>
+          <t>Contradiction</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>AI answers response; Gemini Flash 2.o</t>
+          <t>AI answers response, ChatGPT4o, Claude Sonnet 3.7</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Represent a Client portal for accountants/representatives</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>How My Business Account relates to personal My Account</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>d0e45d52af</t>
+          <t>3899a33225</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>If I am on my Service account, can I access my CRA account?</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>Unique Facts</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
           <t>Claude Sonnet 3.7</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>AI answers response; Gemini Flash 2.o</t>
-        </is>
-      </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Security code mailed to business address must be entered within 45 days</t>
+          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Switch to CRA feature claim (incorrect)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>d0e45d52af</t>
+          <t>3899a33225</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>If I am on my Service account, can I access my CRA account?</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>Unique Facts</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
           <t>ChatGPT4o</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>AI answers response; Gemini Flash 2.o</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Business Number (BN) requirement for registration</t>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Provincial partner sign-in option | Security code mailed after initial registration | CRA contact number 1-800-959-8281</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>d0e45d52af</t>
+          <t>3899a33225</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>If I am on my Service account, can I access my CRA account?</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>Contradiction</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>AI answers response, ChatGPT4o, Claude Sonnet 3.7</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Whether My Business Account is separate from personal My Account or uses same credentials</t>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Ability to navigate from Service Canada account to CRA account</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>3899a33225</t>
+          <t>abed85b806</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>I'm looking for my CRA account sign in page, I only see options to register a new account</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Claude Sonnet 3.7</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
+          <t>AI answers response</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>The 'Switch to CRA' feature exists to navigate between Service Canada and CRA accounts</t>
+          <t>ChatGPT4o; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Mentions provincial partner as a sign-in option | Mentions Represent a Client portal</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>3899a33225</t>
+          <t>abed85b806</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>I'm looking for my CRA account sign in page, I only see options to register a new account</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
+          <t>Unique Facts</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
           <t>ChatGPT4o</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>AI answers response; Gemini Flash 2.o</t>
-        </is>
-      </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Provincial partner sign-in option | Security code mailed to home address for initial registration | CRA contact number 1-800-959-8281 for individuals</t>
+          <t>AI answers response; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Suggests clearing browser cache or using different browser as troubleshooting</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>3899a33225</t>
+          <t>abed85b806</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>I'm looking for my CRA account sign in page, I only see options to register a new account</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t>Unique Facts</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
           <t>Claude Sonnet 3.7</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>ChatGPT4o; Gemini Flash 2.o</t>
-        </is>
-      </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>GCKey as a sign-in method | CRA e-Services Helpdesk number 1-800-959-8281</t>
+          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Mentions GCKey/Government Sign-In option | Provides business account phone number 1-800-959-5525 | Specifically names SecureKey Concierge</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>3899a33225</t>
+          <t>df9c9d8e27</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>my CRA sign in is through my bank and I need to sign in to file my taxes but the CRA Partner sign in is not available</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Claude Sonnet 3.7</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
+          <t>AI answers</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>SecureKey Concierge as the Sign-in Partner service name</t>
+          <t>ChatGPT4o; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Provincial partners (BC Services Card, Alberta.ca Account) as sign-in alternatives</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>3899a33225</t>
+          <t>df9c9d8e27</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Contradiction</t>
+          <t>my CRA sign in is through my bank and I need to sign in to file my taxes but the CRA Partner sign in is not available</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>AI answers response, ChatGPT4o, Claude Sonnet 3.7</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>ChatGPT4o</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Ability to access CRA account from Service Canada account</t>
+          <t>AI answers; Claude Sonnet 3.7; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>System Outages page for checking service status</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>abed85b806</t>
+          <t>df9c9d8e27</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>my CRA sign in is through my bank and I need to sign in to file my taxes but the CRA Partner sign in is not available</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
+          <t>Unique Facts</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
           <t>Claude Sonnet 3.7</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
-        </is>
-      </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>GCKey as a third sign-in option | SecureKey Concierge as the specific name for Sign-in Partner</t>
+          <t>AI answers; ChatGPT4o; Gemini Flash 2.o</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Technical support phone number 1-800-714-7257 | Line 23600 from previous return needed for registration | My Service Canada Account as sign-in alternative</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>abed85b806</t>
+          <t>df9c9d8e27</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Unique Facts</t>
+          <t>my CRA sign in is through my bank and I need to sign in to file my taxes but the CRA Partner sign in is not available</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ChatGPT4o</t>
+          <t>Unique Facts</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>AI answers response; Gemini Flash 2.o</t>
+          <t>Gemini Flash 2.o</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Suggestion to clear browser cache as troubleshooting step</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>abed85b806</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Unique Facts</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Claude Sonnet 3.7</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>Business account phone number 1-800-959-5525</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>abed85b806</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Unique Facts</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>AI answers response</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>ChatGPT4o; Claude Sonnet 3.7; Gemini Flash 2.o</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>Mention of My Business Account and Represent a Client as additional CRA services</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>abed85b806</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Contradiction</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>AI answers response, ChatGPT4o, Claude Sonnet 3.7</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Number of sign-in methods available</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>df9c9d8e27</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Unique Facts</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>AI answers response</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>ChatGPT4o; Claude Sonnet 3.7; Gemini Flash 2.o</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Provincial partner options available (BC Services Card or Alberta.ca Account) | May need to call CRA to revoke old Sign-In Partner before registering new method</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>df9c9d8e27</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Unique Facts</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>ChatGPT4o</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>AI answers response; Claude Sonnet 3.7; Gemini Flash 2.o</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Security code received by mail after CRA registration | System Outages page available for checking service status</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>df9c9d8e27</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Unique Facts</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Claude Sonnet 3.7</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>AI answers response; ChatGPT4o; Gemini Flash 2.o</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>Technical support phone number 1-800-714-7257 | Line 23600 from previous return needed for registration | My Service Canada Account as specific sign-in partner option</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>df9c9d8e27</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Unique Facts</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Gemini Flash 2.o</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>AI answers response; ChatGPT4o; Claude Sonnet 3.7</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>Option to file by mail with paper return | Paper returns have significantly longer processing times</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>df9c9d8e27</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Contradiction</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>AI answers response, ChatGPT4o, Claude Sonnet 3.7</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>Information needed for CRA registration</t>
+          <t>AI answers; ChatGPT4o; Claude Sonnet 3.7</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Paper filing option with forms downloadable or requestable by phone | Try using different financial institution partner if available</t>
         </is>
       </c>
     </row>

</xml_diff>